<commit_message>
Liten update i egen kode
</commit_message>
<xml_diff>
--- a/Arbeidspakker og Timer Vol1.xlsx
+++ b/Arbeidspakker og Timer Vol1.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>Arbeidspakke</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Milestone 1</t>
   </si>
   <si>
-    <t>Dokumentasjon</t>
-  </si>
-  <si>
     <t>Totale timer</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Opprette enkel HTML-side som viser IP-adresse, Sjekke at lastbalansering fungerer</t>
   </si>
   <si>
-    <t xml:space="preserve">Dokumentasjon </t>
-  </si>
-  <si>
     <t>Dokumentasjon av Milestone 3</t>
   </si>
   <si>
@@ -165,10 +159,22 @@
     <t>Faktisk brukte timer</t>
   </si>
   <si>
-    <t>Tre VM-er med Win2012R2 (Script?)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Totalt 3 Win2012R2 servere (1 domenekontroller, 2 resterende meldes inn i domenet) samt teste GPO(Group Policy) og tilangangsstyring </t>
+  </si>
+  <si>
+    <t>Terraform (Første gang)</t>
+  </si>
+  <si>
+    <t>Tre VM-er med Win2012R2 (Script for)</t>
+  </si>
+  <si>
+    <t>Dokumentasjon Milestone 3</t>
+  </si>
+  <si>
+    <t>Dokumentasjon Milestone 2</t>
+  </si>
+  <si>
+    <t>Dokumentasjon Milestone 1</t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +569,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>2</v>
@@ -586,21 +592,20 @@
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6">
-        <f>(7.5+15)*2</f>
-        <v>45</v>
+        <v>37.5</v>
       </c>
       <c r="D2" s="8">
-        <v>45</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -608,21 +613,18 @@
         <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="6">
         <f>(7.5*1)*2</f>
         <v>15</v>
       </c>
-      <c r="D3" s="8">
-        <v>15</v>
-      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -630,7 +632,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6">
         <f>(7.5*2)*2</f>
@@ -646,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -654,12 +656,15 @@
         <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="6">
         <f>(7.5*2)*2</f>
         <v>30</v>
       </c>
+      <c r="D5" s="8">
+        <v>15</v>
+      </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
@@ -667,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -675,20 +680,23 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C6" s="6">
         <f>(7.5*2)*1</f>
         <v>15</v>
       </c>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
       <c r="E6" s="8">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -696,11 +704,11 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6">
-        <f>(7.5*5)*2</f>
-        <v>75</v>
+        <f>(7.5*3)*2</f>
+        <v>45</v>
       </c>
       <c r="E7" s="8">
         <v>2</v>
@@ -709,16 +717,20 @@
         <v>11</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="C8" s="6">
+        <f>(7.5*3)</f>
+        <v>22.5</v>
+      </c>
       <c r="E8" s="8">
         <v>2</v>
       </c>
@@ -726,36 +738,43 @@
         <v>6</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C9" s="6">
+        <f>(7.5*3)</f>
+        <v>22.5</v>
+      </c>
+      <c r="D9" s="8">
+        <f>(7.5*1)</f>
+        <v>7.5</v>
       </c>
       <c r="E9" s="8">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C10" s="6">
-        <f>(7.5*2)*1</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E10" s="8">
         <v>2</v>
@@ -764,15 +783,19 @@
         <v>11</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="6">
+        <f>(7.5*1)*2</f>
+        <v>15</v>
       </c>
       <c r="E11" s="8">
         <v>3</v>
@@ -781,15 +804,19 @@
         <v>11</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C12" s="6">
+        <f>(7.5*2)*2</f>
+        <v>30</v>
       </c>
       <c r="E12" s="8">
         <v>3</v>
@@ -798,32 +825,36 @@
         <v>11</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C13" s="6">
+        <f>(7.5*2)*2</f>
+        <v>30</v>
       </c>
       <c r="E13" s="8">
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C14" s="6">
         <f>(7.5*2)*1</f>
@@ -836,19 +867,19 @@
         <v>11</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="6">
-        <f>(7.5*5)*2</f>
-        <v>75</v>
+        <f>(7.5*1)*2</f>
+        <v>15</v>
       </c>
       <c r="E15" s="8">
         <v>4</v>
@@ -857,15 +888,15 @@
         <v>11</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="6">
         <f>(7.5*2)*2</f>
@@ -878,15 +909,15 @@
         <v>11</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="C17" s="6">
         <f>(7.5*2)*2</f>
@@ -899,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -907,20 +938,20 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6">
         <f>SUM(D2:D19)</f>
-        <v>75</v>
+        <v>75.2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="6">
         <f>SUM(C2:C43)</f>
-        <v>375</v>
+        <v>392.5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -928,7 +959,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="6">
         <v>450</v>
@@ -937,11 +968,11 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="10">
         <f>B25-B23</f>
-        <v>75</v>
+        <v>57.5</v>
       </c>
       <c r="E26" s="8"/>
     </row>
@@ -1166,13 +1197,13 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8595AAA-01C8-4DB9-AB65-E7587227D15B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>